<commit_message>
EPBDS: added check for XmlBeans support
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/OneToOneMappingsTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/OneToOneMappingsTest.xlsx
@@ -4,12 +4,10 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="24735" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="24735" windowHeight="11955"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -144,7 +142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,16 +150,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="56"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="41"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -195,21 +217,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,39 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="H10:H12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="10" spans="8:8">
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="8:8">
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="8:8">
-      <c r="H12" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C4:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -554,309 +569,299 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:9">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="3:9" ht="149.25" customHeight="1">
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="7" spans="3:9">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="3:9" ht="78.75" customHeight="1">
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="12" spans="3:9">
       <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="3:9">
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="3:9">
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="3:9">
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="3:9">
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="3:9">
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2" t="b">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="3:9">
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="2"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="22" spans="3:9">
       <c r="C22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="3:9">
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="3:9">
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="3:9">
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
     </row>
     <row r="26" spans="3:9">
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
     </row>
     <row r="27" spans="3:9">
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="30" spans="3:9">
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="5"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="3:9">
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="32" spans="3:9">
-      <c r="C32" s="5"/>
-      <c r="D32" s="2" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="1" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C12:I12"/>
     <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>